<commit_message>
Update to model data
</commit_message>
<xml_diff>
--- a/Data_Denver_Vaccination_Sites.xlsx
+++ b/Data_Denver_Vaccination_Sites.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sandy Oaks\Documents\Grad School\S21_MATH-7594\Project\COVIDvaccineAllocationIP2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DDD4E58-9D2F-42EA-9088-0156EFD029A5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E044386-5185-49BA-BFC7-3F3DA5A68AC6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{39B1C9AD-B75C-467B-B196-935BFAFEB8D9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{39B1C9AD-B75C-467B-B196-935BFAFEB8D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Service Provider Sites" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="127">
   <si>
     <t>Name</t>
   </si>
@@ -197,9 +197,6 @@
     <t>3800 W 44th Ave Denver, CO 80211</t>
   </si>
   <si>
-    <t>Safeway</t>
-  </si>
-  <si>
     <t>200 Quebec St #400 Denver, CO 80230</t>
   </si>
   <si>
@@ -215,9 +212,6 @@
     <t>2130 Stout St, Denver, CO 80205</t>
   </si>
   <si>
-    <t>Walgreens</t>
-  </si>
-  <si>
     <t>801 16TH ST DENVER, CO 80202</t>
   </si>
   <si>
@@ -305,18 +299,12 @@
     <t>18605 GREEN VALLEY RANCH BLVD Denver, CO 80249</t>
   </si>
   <si>
-    <t>King Soopers</t>
-  </si>
-  <si>
     <t>1000 Chopper Cir, Denver, CO 80204</t>
   </si>
   <si>
     <t>Ball Arena</t>
   </si>
   <si>
-    <t>Dick’s Sporting Good Park</t>
-  </si>
-  <si>
     <t>6000 Victory Way, Commerce City, CO 80022</t>
   </si>
   <si>
@@ -354,6 +342,84 @@
   </si>
   <si>
     <t>max vaccine capacity (f_j), per week</t>
+  </si>
+  <si>
+    <t>King Soopers 1</t>
+  </si>
+  <si>
+    <t>King Soopers 2</t>
+  </si>
+  <si>
+    <t>King Soopers 3</t>
+  </si>
+  <si>
+    <t>King Soopers 4</t>
+  </si>
+  <si>
+    <t>King Soopers 5</t>
+  </si>
+  <si>
+    <t>King Soopers 6</t>
+  </si>
+  <si>
+    <t>King Soopers 7</t>
+  </si>
+  <si>
+    <t>King Soopers 8</t>
+  </si>
+  <si>
+    <t>King Soopers 9</t>
+  </si>
+  <si>
+    <t>King Soopers 10</t>
+  </si>
+  <si>
+    <t>King Soopers 11</t>
+  </si>
+  <si>
+    <t>King Soopers 12</t>
+  </si>
+  <si>
+    <t>King Soopers 13</t>
+  </si>
+  <si>
+    <t>King Soopers 14</t>
+  </si>
+  <si>
+    <t>Safeway 1</t>
+  </si>
+  <si>
+    <t>Safeway 2</t>
+  </si>
+  <si>
+    <t>Walgreens 1</t>
+  </si>
+  <si>
+    <t>Walgreens 2</t>
+  </si>
+  <si>
+    <t>Walgreens 3</t>
+  </si>
+  <si>
+    <t>Walgreens 4</t>
+  </si>
+  <si>
+    <t>Walgreens 5</t>
+  </si>
+  <si>
+    <t>Walgreens 6</t>
+  </si>
+  <si>
+    <t>Walgreens 7</t>
+  </si>
+  <si>
+    <t>Walgreens 8</t>
+  </si>
+  <si>
+    <t>Walgreens 9</t>
+  </si>
+  <si>
+    <t>Dicks Sporting Good Park</t>
   </si>
 </sst>
 </file>
@@ -739,21 +805,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B640664F-C3A9-4269-B5BE-F07F04B3BE01}">
   <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="57" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="45.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="7.77734375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="45.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" style="4" customWidth="1"/>
     <col min="4" max="4" width="7" style="4" customWidth="1"/>
-    <col min="5" max="8" width="60.5546875" style="4" customWidth="1"/>
-    <col min="9" max="16384" width="9.109375" style="4"/>
+    <col min="5" max="8" width="60.5703125" style="4" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -761,30 +827,30 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>21</v>
@@ -796,1060 +862,1060 @@
         <v>-104.908951830685</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="G2" s="4">
-        <v>5</v>
+        <v>5000</v>
       </c>
       <c r="H2" s="4">
         <v>1000</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>90</v>
+        <v>7</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="C3" s="4">
-        <v>39.748681762548799</v>
+        <v>39.788632087137202</v>
       </c>
       <c r="D3" s="4">
-        <v>-105.007774974848</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>89</v>
+        <v>-104.986464364269</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="G3" s="4">
-        <v>30</v>
+        <v>5000</v>
       </c>
       <c r="H3" s="4">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>2</v>
+        <v>1000</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="C4" s="4">
-        <v>39.7199217700269</v>
+        <v>39.643308363688</v>
       </c>
       <c r="D4" s="4">
-        <v>-104.95981893067</v>
+        <v>-105.0336775</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="G4" s="4">
-        <v>15</v>
+        <v>5000</v>
       </c>
       <c r="H4" s="4">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C5" s="4">
-        <v>39.788632087137202</v>
+        <v>39.685224312233899</v>
       </c>
       <c r="D5" s="4">
-        <v>-104.986464364269</v>
+        <v>-105.024505953972</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="G5" s="4">
-        <v>5</v>
+        <v>5000</v>
       </c>
       <c r="H5" s="4">
         <v>1000</v>
       </c>
-      <c r="I5" s="4" t="s">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="4">
+        <v>39.6979323396355</v>
+      </c>
+      <c r="D6" s="4">
+        <v>-104.846263988342</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="G6" s="4">
+        <v>5000</v>
+      </c>
+      <c r="H6" s="4">
+        <v>1000</v>
+      </c>
+      <c r="I6" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="4">
-        <v>39.677733914306103</v>
-      </c>
-      <c r="D6" s="4">
-        <v>-104.909888559824</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="G6" s="4">
-        <v>30</v>
-      </c>
-      <c r="H6" s="4">
-        <v>10000</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C7" s="4">
-        <v>39.643308363688</v>
+        <v>39.692870070623201</v>
       </c>
       <c r="D7" s="4">
-        <v>-105.0336775</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>12</v>
+        <v>-105.02583613068499</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="G7" s="4">
-        <v>5</v>
+        <v>5000</v>
       </c>
       <c r="H7" s="4">
         <v>1000</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I7" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="C8" s="4">
-        <v>39.6551032059443</v>
+        <v>39.756457216795198</v>
       </c>
       <c r="D8" s="4">
-        <v>-104.900764457633</v>
+        <v>-104.975581769314</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="G8" s="4">
-        <v>15</v>
+        <v>5000</v>
       </c>
       <c r="H8" s="4">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C9" s="4">
-        <v>39.728138025292097</v>
+        <v>39.748095057206498</v>
       </c>
       <c r="D9" s="4">
-        <v>-104.991351486459</v>
+        <v>-104.971106284616</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>99</v>
+        <v>32</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>96</v>
       </c>
       <c r="G9" s="4">
-        <v>5</v>
+        <v>5000</v>
       </c>
       <c r="H9" s="4">
-        <v>10000</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C10" s="4">
-        <v>39.685224312233899</v>
+        <v>39.779607493570097</v>
       </c>
       <c r="D10" s="4">
-        <v>-105.024505953972</v>
+        <v>-105.004952846027</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="G10" s="4">
-        <v>5</v>
+        <v>5000</v>
       </c>
       <c r="H10" s="4">
         <v>1000</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I10" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="C11" s="4">
-        <v>39.805843279282598</v>
+        <v>39.730779046180999</v>
       </c>
       <c r="D11" s="4">
-        <v>-104.89185461717599</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>92</v>
+        <v>-104.885742953972</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="G11" s="4">
-        <v>30</v>
+        <v>5000</v>
       </c>
       <c r="H11" s="4">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1000</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C12" s="4">
-        <v>39.6979323396355</v>
+        <v>39.734965348067497</v>
       </c>
       <c r="D12" s="4">
-        <v>-104.846263988342</v>
+        <v>-105.024279715342</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>25</v>
+        <v>71</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="G12" s="4">
-        <v>5</v>
+        <v>5000</v>
       </c>
       <c r="H12" s="4">
         <v>1000</v>
       </c>
-      <c r="I12" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C13" s="4">
-        <v>39.692870070623201</v>
+        <v>39.751290432399401</v>
       </c>
       <c r="D13" s="4">
-        <v>-105.02583613068499</v>
+        <v>-104.986186630685</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="G13" s="4">
-        <v>5</v>
+        <v>5000</v>
       </c>
       <c r="H13" s="4">
         <v>1000</v>
       </c>
-      <c r="I13" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C14" s="4">
-        <v>39.756457216795198</v>
+        <v>39.728138025292097</v>
       </c>
       <c r="D14" s="4">
-        <v>-104.975581769314</v>
+        <v>-104.991351486459</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>100</v>
+        <v>19</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>95</v>
       </c>
       <c r="G14" s="4">
-        <v>5</v>
+        <v>5000</v>
       </c>
       <c r="H14" s="4">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C15" s="4">
-        <v>39.748095057206498</v>
+        <v>39.746855640122099</v>
       </c>
       <c r="D15" s="4">
-        <v>-104.971106284616</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>100</v>
+        <v>-104.964528915342</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>95</v>
       </c>
       <c r="G15" s="4">
-        <v>5</v>
+        <v>5000</v>
       </c>
       <c r="H15" s="4">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C16" s="4">
-        <v>39.746855640122099</v>
+        <v>39.739250354824101</v>
       </c>
       <c r="D16" s="4">
-        <v>-104.964528915342</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>34</v>
+        <v>-104.942420815327</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="G16" s="4">
-        <v>5</v>
+        <v>5000</v>
       </c>
       <c r="H16" s="4">
         <v>10000</v>
       </c>
-      <c r="I16" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="4">
+        <v>39.730894268245798</v>
+      </c>
+      <c r="D17" s="4">
+        <v>-104.934298457594</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G17" s="4">
+        <v>5000</v>
+      </c>
+      <c r="H17" s="4">
+        <v>10000</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="4">
+        <v>39.670765847124997</v>
+      </c>
+      <c r="D18" s="4">
+        <v>-104.97613359205501</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G18" s="4">
+        <v>5000</v>
+      </c>
+      <c r="H18" s="4">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="4">
+        <v>39.746912849039902</v>
+      </c>
+      <c r="D19" s="4">
+        <v>-104.971598015342</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G19" s="4">
+        <v>5000</v>
+      </c>
+      <c r="H19" s="4">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="4">
+        <v>39.748681762548799</v>
+      </c>
+      <c r="D20" s="4">
+        <v>-105.007774974848</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="G20" s="4">
+        <v>30000</v>
+      </c>
+      <c r="H20" s="4">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="4">
+        <v>39.677733914306103</v>
+      </c>
+      <c r="D21" s="4">
+        <v>-104.909888559824</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="G21" s="4">
+        <v>30000</v>
+      </c>
+      <c r="H21" s="4">
+        <v>10000</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="4">
+        <v>39.805843279282598</v>
+      </c>
+      <c r="D22" s="4">
+        <v>-104.89185461717599</v>
+      </c>
+      <c r="E22" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" s="4">
+      <c r="F22" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="G22" s="4">
+        <v>30000</v>
+      </c>
+      <c r="H22" s="4">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="4">
+        <v>39.769548711124102</v>
+      </c>
+      <c r="D23" s="4">
+        <v>-105.008882523286</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G23" s="4">
+        <v>30000</v>
+      </c>
+      <c r="H23" s="4">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="4">
+        <v>39.7199217700269</v>
+      </c>
+      <c r="D24" s="4">
+        <v>-104.95981893067</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G24" s="4">
+        <v>15000</v>
+      </c>
+      <c r="H24" s="4">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="4">
+        <v>39.6551032059443</v>
+      </c>
+      <c r="D25" s="4">
+        <v>-104.900764457633</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G25" s="4">
+        <v>15000</v>
+      </c>
+      <c r="H25" s="4">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="4">
         <v>39.666907554027802</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D26" s="4">
         <v>-104.93674824231501</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E26" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G26" s="4">
+        <v>15000</v>
+      </c>
+      <c r="H26" s="4">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="4">
+        <v>39.737819883861697</v>
+      </c>
+      <c r="D27" s="4">
+        <v>-104.91778233252001</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G27" s="4">
+        <v>15000</v>
+      </c>
+      <c r="H27" s="4">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" s="4">
+        <v>39.679913002392802</v>
+      </c>
+      <c r="D28" s="4">
+        <v>-105.021066456081</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G28" s="4">
+        <v>15000</v>
+      </c>
+      <c r="H28" s="4">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" s="4">
+        <v>39.757126450489601</v>
+      </c>
+      <c r="D29" s="4">
+        <v>-104.99902638834099</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G29" s="4">
+        <v>15000</v>
+      </c>
+      <c r="H29" s="4">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30" s="4">
+        <v>39.759674684394703</v>
+      </c>
+      <c r="D30" s="4">
+        <v>-104.86643017299799</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G30" s="4">
+        <v>15000</v>
+      </c>
+      <c r="H30" s="4">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C31" s="4">
+        <v>39.785448614830699</v>
+      </c>
+      <c r="D31" s="4">
+        <v>-104.77017538833999</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G31" s="4">
+        <v>15000</v>
+      </c>
+      <c r="H31" s="4">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32" s="4">
+        <v>39.731279102110101</v>
+      </c>
+      <c r="D32" s="4">
+        <v>-104.97358613252</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G32" s="4">
+        <v>15000</v>
+      </c>
+      <c r="H32" s="4">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33" s="4">
+        <v>39.756675945226199</v>
+      </c>
+      <c r="D33" s="4">
+        <v>-104.90174819231299</v>
+      </c>
+      <c r="E33" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="F17" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="G17" s="4">
-        <v>15</v>
-      </c>
-      <c r="H17" s="4">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18" s="4">
-        <v>39.731279102110101</v>
-      </c>
-      <c r="D18" s="4">
-        <v>-104.97358613252</v>
-      </c>
-      <c r="E18" s="4" t="s">
+      <c r="F33" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G33" s="4">
+        <v>15000</v>
+      </c>
+      <c r="H33" s="4">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C34" s="4">
+        <v>39.737702485194198</v>
+      </c>
+      <c r="D34" s="4">
+        <v>-104.997936272999</v>
+      </c>
+      <c r="E34" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="F18" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="G18" s="4">
-        <v>15</v>
-      </c>
-      <c r="H18" s="4">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C19" s="4">
-        <v>39.756675945226199</v>
-      </c>
-      <c r="D19" s="4">
-        <v>-104.90174819231299</v>
-      </c>
-      <c r="E19" s="4" t="s">
+      <c r="F34" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G34" s="4">
+        <v>15000</v>
+      </c>
+      <c r="H34" s="4">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" s="4">
+        <v>39.690880684958898</v>
+      </c>
+      <c r="D35" s="4">
+        <v>-105.05212807300001</v>
+      </c>
+      <c r="E35" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="F19" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="G19" s="4">
-        <v>15</v>
-      </c>
-      <c r="H19" s="4">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C20" s="4">
-        <v>39.737702485194198</v>
-      </c>
-      <c r="D20" s="4">
-        <v>-104.997936272999</v>
-      </c>
-      <c r="E20" s="4" t="s">
+      <c r="F35" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G35" s="4">
+        <v>15000</v>
+      </c>
+      <c r="H35" s="4">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" s="4">
+        <v>39.654780462643402</v>
+      </c>
+      <c r="D36" s="4">
+        <v>-105.051212746014</v>
+      </c>
+      <c r="E36" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="F20" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="G20" s="4">
-        <v>15</v>
-      </c>
-      <c r="H20" s="4">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C21" s="4">
-        <v>39.690880684958898</v>
-      </c>
-      <c r="D21" s="4">
-        <v>-105.05212807300001</v>
-      </c>
-      <c r="E21" s="4" t="s">
+      <c r="F36" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G36" s="4">
+        <v>15000</v>
+      </c>
+      <c r="H36" s="4">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C37" s="4">
+        <v>39.652072265935402</v>
+      </c>
+      <c r="D37" s="4">
+        <v>-104.91423037485001</v>
+      </c>
+      <c r="E37" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="F21" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="G21" s="4">
-        <v>15</v>
-      </c>
-      <c r="H21" s="4">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C22" s="4">
-        <v>39.654780462643402</v>
-      </c>
-      <c r="D22" s="4">
-        <v>-105.051212746014</v>
-      </c>
-      <c r="E22" s="4" t="s">
+      <c r="F37" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G37" s="4">
+        <v>15000</v>
+      </c>
+      <c r="H37" s="4">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" s="4">
+        <v>39.701141398944102</v>
+      </c>
+      <c r="D38" s="4">
+        <v>-104.911359188342</v>
+      </c>
+      <c r="E38" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="F22" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="G22" s="4">
-        <v>15</v>
-      </c>
-      <c r="H22" s="4">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C23" s="4">
-        <v>39.652072265935402</v>
-      </c>
-      <c r="D23" s="4">
-        <v>-104.91423037485001</v>
-      </c>
-      <c r="E23" s="4" t="s">
+      <c r="F38" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G38" s="4">
+        <v>15000</v>
+      </c>
+      <c r="H38" s="4">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C39" s="4">
+        <v>39.7022968513729</v>
+      </c>
+      <c r="D39" s="4">
+        <v>-104.941461986492</v>
+      </c>
+      <c r="E39" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="F23" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="G23" s="4">
-        <v>15</v>
-      </c>
-      <c r="H23" s="4">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C24" s="4">
-        <v>39.701141398944102</v>
-      </c>
-      <c r="D24" s="4">
-        <v>-104.911359188342</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="G24" s="4">
-        <v>15</v>
-      </c>
-      <c r="H24" s="4">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C25" s="4">
-        <v>39.7022968513729</v>
-      </c>
-      <c r="D25" s="4">
-        <v>-104.941461986492</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="G25" s="4">
-        <v>15</v>
-      </c>
-      <c r="H25" s="4">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C26" s="4">
-        <v>39.737819883861697</v>
-      </c>
-      <c r="D26" s="4">
-        <v>-104.91778233252001</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="G26" s="4">
-        <v>15</v>
-      </c>
-      <c r="H26" s="4">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C27" s="4">
-        <v>39.679913002392802</v>
-      </c>
-      <c r="D27" s="4">
-        <v>-105.021066456081</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="G27" s="4">
-        <v>15</v>
-      </c>
-      <c r="H27" s="4">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C28" s="4">
-        <v>39.757126450489601</v>
-      </c>
-      <c r="D28" s="4">
-        <v>-104.99902638834099</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="G28" s="4">
-        <v>15</v>
-      </c>
-      <c r="H28" s="4">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C29" s="4">
-        <v>39.759674684394703</v>
-      </c>
-      <c r="D29" s="4">
-        <v>-104.86643017299799</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="G29" s="4">
-        <v>15</v>
-      </c>
-      <c r="H29" s="4">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C30" s="4">
-        <v>39.785448614830699</v>
-      </c>
-      <c r="D30" s="4">
-        <v>-104.77017538833999</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="G30" s="4">
-        <v>15</v>
-      </c>
-      <c r="H30" s="4">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C31" s="4">
-        <v>39.779607493570097</v>
-      </c>
-      <c r="D31" s="4">
-        <v>-105.004952846027</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="G31" s="4">
-        <v>5</v>
-      </c>
-      <c r="H31" s="4">
-        <v>1000</v>
-      </c>
-      <c r="I31" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C32" s="4">
-        <v>39.769548711124102</v>
-      </c>
-      <c r="D32" s="4">
-        <v>-105.008882523286</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="G32" s="4">
-        <v>30</v>
-      </c>
-      <c r="H32" s="4">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C33" s="4">
-        <v>39.730779046180999</v>
-      </c>
-      <c r="D33" s="4">
-        <v>-104.885742953972</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="G33" s="4">
-        <v>5</v>
-      </c>
-      <c r="H33" s="4">
-        <v>1000</v>
-      </c>
-      <c r="I33" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C34" s="4">
-        <v>39.739250354824101</v>
-      </c>
-      <c r="D34" s="4">
-        <v>-104.942420815327</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="G34" s="4">
-        <v>5</v>
-      </c>
-      <c r="H34" s="4">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C35" s="4">
-        <v>39.730894268245798</v>
-      </c>
-      <c r="D35" s="4">
-        <v>-104.934298457594</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="G35" s="4">
-        <v>5</v>
-      </c>
-      <c r="H35" s="4">
-        <v>10000</v>
-      </c>
-      <c r="I35" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C36" s="4">
-        <v>39.670765847124997</v>
-      </c>
-      <c r="D36" s="4">
-        <v>-104.97613359205501</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="G36" s="4">
-        <v>5</v>
-      </c>
-      <c r="H36" s="4">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
+      <c r="F39" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G39" s="4">
+        <v>15000</v>
+      </c>
+      <c r="H39" s="4">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C40" s="4">
+        <v>39.776267991208101</v>
+      </c>
+      <c r="D40" s="4">
+        <v>-105.036376696055</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G40" s="4">
+        <v>15000</v>
+      </c>
+      <c r="H40" s="4">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C41" s="4">
+        <v>39.720484964228</v>
+      </c>
+      <c r="D41" s="4">
+        <v>-104.901111601835</v>
+      </c>
+      <c r="E41" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B37" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C37" s="4">
-        <v>39.776267991208101</v>
-      </c>
-      <c r="D37" s="4">
-        <v>-105.036376696055</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="G37" s="4">
-        <v>15</v>
-      </c>
-      <c r="H37" s="4">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C38" s="4">
-        <v>39.720484964228</v>
-      </c>
-      <c r="D38" s="4">
-        <v>-104.901111601835</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="F38" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="G38" s="4">
-        <v>15</v>
-      </c>
-      <c r="H38" s="4">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C39" s="4">
-        <v>39.746912849039902</v>
-      </c>
-      <c r="D39" s="4">
-        <v>-104.971598015342</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="G39" s="4">
-        <v>5</v>
-      </c>
-      <c r="H39" s="4">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C40" s="4">
-        <v>39.734965348067497</v>
-      </c>
-      <c r="D40" s="4">
-        <v>-105.024279715342</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="F40" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="G40" s="4">
-        <v>5</v>
-      </c>
-      <c r="H40" s="4">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C41" s="4">
-        <v>39.751290432399401</v>
-      </c>
-      <c r="D41" s="4">
-        <v>-104.986186630685</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="F41" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G41" s="4">
-        <v>5</v>
+        <v>15000</v>
       </c>
       <c r="H41" s="4">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>42</v>
       </c>
@@ -1866,18 +1932,18 @@
         <v>43</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="G42" s="4">
-        <v>15</v>
+        <v>15000</v>
       </c>
       <c r="H42" s="4">
         <v>300</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
-        <v>58</v>
+        <v>117</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>3</v>
@@ -1889,21 +1955,21 @@
         <v>-104.993051532519</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="G43" s="4">
-        <v>15</v>
+        <v>15000</v>
       </c>
       <c r="H43" s="4">
         <v>300</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>58</v>
+        <v>118</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>3</v>
@@ -1915,21 +1981,21 @@
         <v>-105.025817359505</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="G44" s="4">
-        <v>15</v>
+        <v>15000</v>
       </c>
       <c r="H44" s="4">
         <v>300</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
-        <v>58</v>
+        <v>119</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>3</v>
@@ -1941,21 +2007,21 @@
         <v>-104.96304463067</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="G45" s="4">
-        <v>15</v>
+        <v>15000</v>
       </c>
       <c r="H45" s="4">
         <v>300</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
-        <v>58</v>
+        <v>120</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>3</v>
@@ -1967,21 +2033,21 @@
         <v>-104.98713463067</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="G46" s="4">
-        <v>15</v>
+        <v>15000</v>
       </c>
       <c r="H46" s="4">
         <v>300</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
-        <v>58</v>
+        <v>121</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>3</v>
@@ -1993,21 +2059,21 @@
         <v>-105.05238385950599</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="G47" s="4">
-        <v>15</v>
+        <v>15000</v>
       </c>
       <c r="H47" s="4">
         <v>300</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
-        <v>58</v>
+        <v>122</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>3</v>
@@ -2019,21 +2085,21 @@
         <v>-104.941016588341</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="G48" s="4">
-        <v>15</v>
+        <v>15000</v>
       </c>
       <c r="H48" s="4">
         <v>300</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
-        <v>58</v>
+        <v>123</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>3</v>
@@ -2045,21 +2111,21 @@
         <v>-105.024524399985</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="G49" s="4">
-        <v>15</v>
+        <v>15000</v>
       </c>
       <c r="H49" s="4">
         <v>300</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
-        <v>58</v>
+        <v>124</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>3</v>
@@ -2071,21 +2137,21 @@
         <v>-104.915572686492</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="G50" s="4">
-        <v>15</v>
+        <v>15000</v>
       </c>
       <c r="H50" s="4">
         <v>300</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
-        <v>58</v>
+        <v>125</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>3</v>
@@ -2097,21 +2163,21 @@
         <v>-104.939545659506</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="G51" s="4">
-        <v>15</v>
+        <v>15000</v>
       </c>
       <c r="H51" s="4">
         <v>300</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>3</v>
@@ -2123,21 +2189,21 @@
         <v>-104.889752530671</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="G52" s="4">
-        <v>15</v>
+        <v>15000</v>
       </c>
       <c r="H52" s="4">
         <v>300</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>3</v>
@@ -2149,13 +2215,13 @@
         <v>-105.02159947299999</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="G53" s="4">
-        <v>15</v>
+        <v>15000</v>
       </c>
       <c r="H53" s="4">
         <v>300</v>
@@ -2164,7 +2230,7 @@
   </sheetData>
   <autoFilter ref="A1:I53" xr:uid="{2B2DFF4D-D60D-48F8-B3B1-546A46E9CAAF}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I53">
-      <sortCondition ref="A1:A52"/>
+      <sortCondition ref="B1:B53"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2180,12 +2246,12 @@
       <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="52.6640625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="52.7109375" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="4">
         <v>39.699406781944802</v>
       </c>
@@ -2193,7 +2259,7 @@
         <v>-104.908951830685</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>39.748681762548799</v>
       </c>
@@ -2201,7 +2267,7 @@
         <v>-105.007774974848</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>39.7199217700269</v>
       </c>
@@ -2209,7 +2275,7 @@
         <v>-104.95981893067</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>39.788632087137202</v>
       </c>
@@ -2217,7 +2283,7 @@
         <v>-104.986464364269</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>39.677733914306103</v>
       </c>
@@ -2225,7 +2291,7 @@
         <v>-104.909888559824</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>39.643308363688</v>
       </c>
@@ -2233,7 +2299,7 @@
         <v>-105.0336775</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>39.6551032059443</v>
       </c>
@@ -2241,7 +2307,7 @@
         <v>-104.900764457633</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>39.728138025292097</v>
       </c>
@@ -2249,7 +2315,7 @@
         <v>-104.991351486459</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>39.685224312233899</v>
       </c>
@@ -2257,7 +2323,7 @@
         <v>-105.024505953972</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>39.805843279282598</v>
       </c>
@@ -2265,7 +2331,7 @@
         <v>-104.89185461717599</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>39.6979323396355</v>
       </c>
@@ -2273,7 +2339,7 @@
         <v>-104.846263988342</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>39.692870070623201</v>
       </c>
@@ -2281,7 +2347,7 @@
         <v>-105.02583613068499</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>39.756457216795198</v>
       </c>
@@ -2289,7 +2355,7 @@
         <v>-104.975581769314</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>39.748095057206498</v>
       </c>
@@ -2297,7 +2363,7 @@
         <v>-104.971106284616</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>39.746855640122099</v>
       </c>
@@ -2305,7 +2371,7 @@
         <v>-104.964528915342</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>39.666907554027802</v>
       </c>
@@ -2313,7 +2379,7 @@
         <v>-104.93674824231501</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>39.731279102110101</v>
       </c>
@@ -2321,7 +2387,7 @@
         <v>-104.97358613252</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>39.756675945226199</v>
       </c>
@@ -2329,7 +2395,7 @@
         <v>-104.90174819231299</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>39.737702485194198</v>
       </c>
@@ -2337,7 +2403,7 @@
         <v>-104.997936272999</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>39.690880684958898</v>
       </c>
@@ -2345,7 +2411,7 @@
         <v>-105.05212807300001</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>39.654780462643402</v>
       </c>
@@ -2353,7 +2419,7 @@
         <v>-105.051212746014</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>39.652072265935402</v>
       </c>
@@ -2361,7 +2427,7 @@
         <v>-104.91423037485001</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>39.701141398944102</v>
       </c>
@@ -2369,7 +2435,7 @@
         <v>-104.911359188342</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>39.7022968513729</v>
       </c>
@@ -2377,7 +2443,7 @@
         <v>-104.941461986492</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>39.737819883861697</v>
       </c>
@@ -2385,7 +2451,7 @@
         <v>-104.91778233252001</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>39.679913002392802</v>
       </c>
@@ -2393,7 +2459,7 @@
         <v>-105.021066456081</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>39.757126450489601</v>
       </c>
@@ -2401,7 +2467,7 @@
         <v>-104.99902638834099</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>39.759674684394703</v>
       </c>
@@ -2409,7 +2475,7 @@
         <v>-104.86643017299799</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>39.785448614830699</v>
       </c>
@@ -2417,7 +2483,7 @@
         <v>-104.77017538833999</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>39.779607493570097</v>
       </c>
@@ -2425,7 +2491,7 @@
         <v>-105.004952846027</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>39.769548711124102</v>
       </c>
@@ -2433,7 +2499,7 @@
         <v>-105.008882523286</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>39.730779046180999</v>
       </c>
@@ -2441,7 +2507,7 @@
         <v>-104.885742953972</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>39.739250354824101</v>
       </c>
@@ -2449,7 +2515,7 @@
         <v>-104.942420815327</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>39.730894268245798</v>
       </c>
@@ -2457,7 +2523,7 @@
         <v>-104.934298457594</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>39.670765847124997</v>
       </c>
@@ -2465,7 +2531,7 @@
         <v>-104.97613359205501</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>39.776267991208101</v>
       </c>
@@ -2473,7 +2539,7 @@
         <v>-105.036376696055</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>39.720484964228</v>
       </c>
@@ -2481,7 +2547,7 @@
         <v>-104.901111601835</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>39.746912849039902</v>
       </c>
@@ -2489,7 +2555,7 @@
         <v>-104.971598015342</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>39.734965348067497</v>
       </c>
@@ -2497,7 +2563,7 @@
         <v>-105.024279715342</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>39.751290432399401</v>
       </c>
@@ -2505,7 +2571,7 @@
         <v>-104.986186630685</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>39.735716247906403</v>
       </c>
@@ -2513,7 +2579,7 @@
         <v>-104.93567523068501</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>39.746391266936598</v>
       </c>
@@ -2521,7 +2587,7 @@
         <v>-104.993051532519</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>39.760138145439498</v>
       </c>
@@ -2529,7 +2595,7 @@
         <v>-105.025817359505</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>39.739779179570597</v>
       </c>
@@ -2537,7 +2603,7 @@
         <v>-104.96304463067</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>39.718989971922497</v>
       </c>
@@ -2545,7 +2611,7 @@
         <v>-104.98713463067</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>39.7408603269838</v>
       </c>
@@ -2553,7 +2619,7 @@
         <v>-105.05238385950599</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>39.766710061976703</v>
       </c>
@@ -2561,7 +2627,7 @@
         <v>-104.941016588341</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>39.711030222751504</v>
       </c>
@@ -2569,7 +2635,7 @@
         <v>-105.024524399985</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>39.7396769801435</v>
       </c>
@@ -2577,7 +2643,7 @@
         <v>-104.915572686492</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>39.7105346172984</v>
       </c>
@@ -2585,7 +2651,7 @@
         <v>-104.939545659506</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
         <v>39.690753085233602</v>
       </c>
@@ -2593,7 +2659,7 @@
         <v>-104.889752530671</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
         <v>39.677884542636001</v>
       </c>
@@ -2612,7 +2678,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>